<commit_message>
Update code and metadata
</commit_message>
<xml_diff>
--- a/Barnes et al Metadata.xlsx
+++ b/Barnes et al Metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://waikatouniversitynz-my.sharepoint.com/personal/andrew_barnes_waikato_ac_nz/Documents/FuSED/BEF-in-Food-Webs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{D7D2BF12-2168-4BC9-A61A-666DFCE47B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1665744A-CED4-42EA-A6E3-06626E3B8024}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{D7D2BF12-2168-4BC9-A61A-666DFCE47B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F140B2F6-CF89-45ED-9975-1082C095CA91}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D124D73A-4991-4D5F-A5DE-0937E14EF04C}"/>
+    <workbookView xWindow="59505" yWindow="825" windowWidth="21600" windowHeight="11175" xr2:uid="{D124D73A-4991-4D5F-A5DE-0937E14EF04C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>ecosystem.type</t>
   </si>
@@ -156,12 +156,60 @@
   <si>
     <t>The leading eigenvalue of the Jacobian matrix</t>
   </si>
+  <si>
+    <t>PC.predation</t>
+  </si>
+  <si>
+    <t>density</t>
+  </si>
+  <si>
+    <t>metric</t>
+  </si>
+  <si>
+    <t>NPP.proxy</t>
+  </si>
+  <si>
+    <t>NPP.scale</t>
+  </si>
+  <si>
+    <t>NPP.scale2</t>
+  </si>
+  <si>
+    <t>measure of NPP (NDVI or chlorophyll-a)</t>
+  </si>
+  <si>
+    <t>Raw NPP value derived from metric</t>
+  </si>
+  <si>
+    <t>Estimated consumer density (abundance/area) of the food web</t>
+  </si>
+  <si>
+    <t>logit-transformed NPP.proxy</t>
+  </si>
+  <si>
+    <t>NPP.scale^2 (quadratic term)</t>
+  </si>
+  <si>
+    <r>
+      <t>Per capita</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> predation rate (prey outflux / prey biomass)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +230,14 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,9 +260,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -541,15 +598,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37DD91D-93F3-461D-96AE-FE7E8FBC8FCF}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -579,50 +636,50 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
@@ -659,42 +716,90 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>